<commit_message>
solved **task for eighth lesson
</commit_message>
<xml_diff>
--- a/less8/table.xlsx
+++ b/less8/table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
@@ -16,13 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>[0,0 *0,0]+[0,1*1,0]</t>
-  </si>
-  <si>
-    <t>[0,0*0,1]+[0,1*1,1]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>[0,0*0,2]+[0,1*1,2]</t>
   </si>
@@ -44,12 +38,157 @@
   <si>
     <t>[2,0 *0,2]+[2,1*1,2]</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 *0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">] + [ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 *1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0]</t>
+    </r>
+  </si>
+  <si>
+    <t>[i,0*0,j]+[i,1*1,j]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +221,46 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,13 +385,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,19 +418,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -323,6 +508,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -357,6 +543,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -532,50 +719,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:28" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:28" ht="31.5">
-      <c r="B2" s="2"/>
-      <c r="C2" s="3">
+    <row r="1" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:28" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="6">
         <v>0</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="3">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="6">
         <v>1</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="3">
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="6">
         <v>2</v>
       </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="5"/>
-      <c r="W2" s="1">
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="8"/>
+      <c r="W2" s="5">
         <v>3</v>
       </c>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1">
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5">
         <v>6</v>
       </c>
-      <c r="Z2" s="1"/>
+      <c r="Z2" s="5"/>
       <c r="AA2">
         <v>3</v>
       </c>
@@ -583,30 +770,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:28" ht="32.25" thickBot="1">
-      <c r="B3" s="2"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="8"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
+    <row r="3" spans="2:28" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
       <c r="AA3">
         <v>2</v>
       </c>
@@ -614,232 +801,233 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:28" ht="31.5" customHeight="1">
-      <c r="B4" s="9">
+    <row r="4" spans="2:28" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="3" t="s">
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="8"/>
+      <c r="W4" s="5">
         <v>1</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="3" t="s">
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z4" s="5"/>
+    </row>
+    <row r="5" spans="2:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="11"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+    </row>
+    <row r="6" spans="2:28" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="5"/>
-      <c r="W4" s="1">
-        <v>1</v>
-      </c>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1">
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="8"/>
+      <c r="W6" s="5">
+        <v>5</v>
+      </c>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5">
+        <v>8</v>
+      </c>
+      <c r="Z6" s="5"/>
+    </row>
+    <row r="7" spans="2:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="4"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="11"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+    </row>
+    <row r="8" spans="2:28" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="2:28" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B5" s="10"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="8"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="2:28" ht="31.5" customHeight="1">
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="8"/>
+    </row>
+    <row r="9" spans="2:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="11"/>
+      <c r="W9" s="5">
+        <v>7</v>
+      </c>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5">
+        <v>9</v>
+      </c>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="5"/>
+    </row>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="W11" s="5">
+        <v>6</v>
+      </c>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="5"/>
-      <c r="W6" s="1">
-        <v>5</v>
-      </c>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1">
-        <v>8</v>
-      </c>
-      <c r="Z6" s="1"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B7" s="10"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="8"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-    </row>
-    <row r="8" spans="2:28" ht="31.5" customHeight="1">
-      <c r="B8" s="9">
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5">
         <v>2</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="3" t="s">
+      <c r="AB11" s="5"/>
+    </row>
+    <row r="12" spans="2:28" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="5"/>
-    </row>
-    <row r="9" spans="2:28" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B9" s="10"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="8"/>
-      <c r="W9" s="1">
-        <v>7</v>
-      </c>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1">
-        <v>9</v>
-      </c>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="1"/>
-    </row>
-    <row r="10" spans="2:28">
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-    </row>
-    <row r="11" spans="2:28">
-      <c r="W11" s="1">
-        <v>6</v>
-      </c>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1">
-        <v>3</v>
-      </c>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1">
-        <v>2</v>
-      </c>
-      <c r="AB11" s="1"/>
-    </row>
-    <row r="12" spans="2:28">
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-    </row>
-    <row r="14" spans="2:28">
-      <c r="S14" s="11"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5"/>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="S14" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="W9:X10"/>
-    <mergeCell ref="Y9:Z10"/>
+    <mergeCell ref="I2:N3"/>
+    <mergeCell ref="O2:T3"/>
+    <mergeCell ref="C2:H3"/>
     <mergeCell ref="AA9:AB10"/>
     <mergeCell ref="W11:X12"/>
     <mergeCell ref="Y11:Z12"/>
@@ -850,6 +1038,11 @@
     <mergeCell ref="Y4:Z5"/>
     <mergeCell ref="Y6:Z7"/>
     <mergeCell ref="W6:X7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="W9:X10"/>
+    <mergeCell ref="Y9:Z10"/>
     <mergeCell ref="C4:H5"/>
     <mergeCell ref="I4:N5"/>
     <mergeCell ref="O4:T5"/>
@@ -859,9 +1052,6 @@
     <mergeCell ref="I8:N9"/>
     <mergeCell ref="O6:T7"/>
     <mergeCell ref="O8:T9"/>
-    <mergeCell ref="I2:N3"/>
-    <mergeCell ref="O2:T3"/>
-    <mergeCell ref="C2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -869,12 +1059,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -882,12 +1072,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>